<commit_message>
Adapted CS+ and CS+ consequences
</commit_message>
<xml_diff>
--- a/chooseBlockA.xlsx
+++ b/chooseBlockA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sag22id\Documents\Projects\GCA\gaze_avoidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4BCB14-610D-48AC-8754-A9A0EE9FF19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A0F4DB-575D-49D6-9031-0FE6D93A6B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14700" yWindow="471" windowWidth="14383" windowHeight="8658" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
+    <workbookView xWindow="-31311" yWindow="3789" windowWidth="14382" windowHeight="9814" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>cs_plus</t>
-  </si>
-  <si>
-    <t>cs_minus</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>stimuli/social/016_y_m_n_b.jpg</t>
   </si>
@@ -62,13 +56,22 @@
     <t>positions.xlsx</t>
   </si>
   <si>
-    <t>blockType</t>
-  </si>
-  <si>
-    <t>social</t>
-  </si>
-  <si>
-    <t>non-social</t>
+    <t>cs_plus_s</t>
+  </si>
+  <si>
+    <t>cs_plus_ns</t>
+  </si>
+  <si>
+    <t>cs_minus_s</t>
+  </si>
+  <si>
+    <t>cs_minus_ns</t>
+  </si>
+  <si>
+    <t>stimFile</t>
+  </si>
+  <si>
+    <t>stimuli.xlsx</t>
   </si>
 </sst>
 </file>
@@ -420,59 +423,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D442166-CB98-4944-BF44-DA0360414B46}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.53515625" customWidth="1"/>
     <col min="3" max="3" width="40.84375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.84375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete visual_clutter and restructure stimulus folder
</commit_message>
<xml_diff>
--- a/chooseBlockA.xlsx
+++ b/chooseBlockA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sag22id\Documents\Projects\GCA\gaze_avoidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A0F4DB-575D-49D6-9031-0FE6D93A6B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B7C7A8-D171-422E-9966-25DFA1AF88E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31311" yWindow="3789" windowWidth="14382" windowHeight="9814" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="8957" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,18 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>stimuli/social/016_y_m_n_b.jpg</t>
-  </si>
-  <si>
-    <t>stimuli/social/031_y_m_n_a.jpg</t>
-  </si>
-  <si>
-    <t>stimuli/non-social/016_y_m_n_b_scrambled.jpg</t>
-  </si>
-  <si>
-    <t>stimuli/non-social/031_y_m_n_a_scrambled.jpg</t>
-  </si>
-  <si>
     <t>posFile</t>
   </si>
   <si>
@@ -72,6 +60,18 @@
   </si>
   <si>
     <t>stimuli.xlsx</t>
+  </si>
+  <si>
+    <t>stimuli/Social1.png</t>
+  </si>
+  <si>
+    <t>stimuli/Social2.png</t>
+  </si>
+  <si>
+    <t>stimuli/Nonsocial1.png</t>
+  </si>
+  <si>
+    <t>stimuli/Nonsocial2.png</t>
   </si>
 </sst>
 </file>
@@ -426,57 +426,55 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="16.53515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.53515625" customWidth="1"/>
-    <col min="3" max="3" width="40.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.84375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adapted stimulus size and bugfix regarding recording of eye-tracking
</commit_message>
<xml_diff>
--- a/chooseBlockA.xlsx
+++ b/chooseBlockA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sag22id\Documents\Projects\GCA\gaze_avoidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B7C7A8-D171-422E-9966-25DFA1AF88E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CDD12E-D9D1-413E-B174-10B210852B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="8957" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>